<commit_message>
Finished building loading Added images for resources
</commit_message>
<xml_diff>
--- a/4xCityBuilder/Assets/Definitions/Buildings.xlsx
+++ b/4xCityBuilder/Assets/Definitions/Buildings.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAC3179-67C2-4395-8AD7-70FE76D99A57}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67969BEE-104E-4681-9646-1F193D069EED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18315" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="87">
   <si>
     <t>Tier</t>
   </si>
   <si>
-    <t>Resource Count to Build</t>
-  </si>
-  <si>
     <t>Job Name</t>
   </si>
   <si>
@@ -40,9 +37,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Resource Category to Build</t>
-  </si>
-  <si>
     <t>Min Resource Tier</t>
   </si>
   <si>
@@ -133,12 +127,6 @@
     <t>Precious Metal</t>
   </si>
   <si>
-    <t>Iron</t>
-  </si>
-  <si>
-    <t>Gold</t>
-  </si>
-  <si>
     <t>Advanced Smelter</t>
   </si>
   <si>
@@ -269,6 +257,30 @@
   </si>
   <si>
     <t>Armorsmith</t>
+  </si>
+  <si>
+    <t>Resource Type to Build</t>
+  </si>
+  <si>
+    <t>Resource Count</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Textures/Buildings/Hut</t>
+  </si>
+  <si>
+    <t>Textures/Buildings/RudimentaryMine</t>
+  </si>
+  <si>
+    <t>Textures/Buildings/RudimentaryForge</t>
+  </si>
+  <si>
+    <t>Textures/Buildings/RudimentaryWeaponsmith</t>
+  </si>
+  <si>
+    <t>Textures/Buildings/RudimentaryArmorsmith</t>
   </si>
 </sst>
 </file>
@@ -601,13 +613,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S69"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="T52" sqref="T52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,86 +641,89 @@
     <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
       </c>
       <c r="M2">
         <v>100</v>
@@ -719,34 +734,37 @@
       <c r="R2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>13</v>
-      </c>
-      <c r="K3" t="s">
-        <v>15</v>
       </c>
       <c r="L3">
         <v>10</v>
@@ -761,9 +779,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -772,18 +790,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -792,13 +810,13 @@
         <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
         <v>13</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
       </c>
       <c r="L5">
         <v>15</v>
@@ -813,9 +831,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -824,9 +842,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -835,18 +853,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -855,7 +873,7 @@
         <v>5</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M8">
         <v>100</v>
@@ -864,10 +882,10 @@
         <v>5</v>
       </c>
       <c r="P8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -875,42 +893,45 @@
       <c r="S8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" t="s">
-        <v>45</v>
-      </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L10">
         <v>50</v>
@@ -922,10 +943,10 @@
         <v>10</v>
       </c>
       <c r="P10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -934,9 +955,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -945,21 +966,21 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -968,10 +989,10 @@
         <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M12">
         <v>100</v>
@@ -980,10 +1001,10 @@
         <v>5</v>
       </c>
       <c r="P12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="R12">
         <v>1</v>
@@ -992,18 +1013,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1012,13 +1033,13 @@
         <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L13">
         <v>50</v>
@@ -1030,10 +1051,10 @@
         <v>10</v>
       </c>
       <c r="P13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="R13">
         <v>2</v>
@@ -1042,9 +1063,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -1053,18 +1074,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1073,13 +1094,13 @@
         <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J15" s="2">
         <v>2</v>
       </c>
       <c r="K15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L15">
         <v>-50</v>
@@ -1091,18 +1112,18 @@
         <v>5</v>
       </c>
       <c r="P15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="R15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1111,13 +1132,13 @@
         <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J16" s="2">
         <v>2</v>
       </c>
       <c r="K16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L16">
         <v>-50</v>
@@ -1125,7 +1146,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1136,16 +1157,16 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1154,16 +1175,16 @@
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J18" s="2">
         <v>3</v>
       </c>
       <c r="K18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1175,10 +1196,10 @@
         <v>10</v>
       </c>
       <c r="P18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="R18">
         <v>2</v>
@@ -1186,7 +1207,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1195,13 +1216,13 @@
         <v>20</v>
       </c>
       <c r="I19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J19" s="2">
         <v>3</v>
       </c>
       <c r="K19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1209,7 +1230,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1220,7 +1241,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1231,16 +1252,16 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1249,19 +1270,19 @@
         <v>50</v>
       </c>
       <c r="G22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J22" s="2">
         <v>4</v>
       </c>
       <c r="K22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L22">
         <v>50</v>
@@ -1273,10 +1294,10 @@
         <v>15</v>
       </c>
       <c r="P22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="R22">
         <v>3</v>
@@ -1284,7 +1305,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -1293,13 +1314,13 @@
         <v>50</v>
       </c>
       <c r="I23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J23" s="2">
         <v>4</v>
       </c>
       <c r="K23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L23">
         <v>50</v>
@@ -1307,7 +1328,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1318,7 +1339,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1329,33 +1350,33 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
       </c>
       <c r="F26">
         <v>25</v>
       </c>
       <c r="P26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -1364,19 +1385,19 @@
         <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J27" s="2">
         <v>5</v>
       </c>
       <c r="K27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L27">
         <v>100</v>
@@ -1393,7 +1414,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -1402,13 +1423,13 @@
         <v>100</v>
       </c>
       <c r="I28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J28" s="2">
         <v>5</v>
       </c>
       <c r="K28" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L28">
         <v>100</v>
@@ -1416,7 +1437,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1427,7 +1448,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1438,10 +1459,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
       </c>
       <c r="F31">
         <v>50</v>
@@ -1449,16 +1470,16 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B32">
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -1467,19 +1488,19 @@
         <v>100</v>
       </c>
       <c r="G32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" t="s">
         <v>39</v>
-      </c>
-      <c r="H32" t="s">
-        <v>45</v>
-      </c>
-      <c r="I32" t="s">
-        <v>43</v>
       </c>
       <c r="J32" s="2">
         <v>5</v>
       </c>
       <c r="K32" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L32">
         <v>100</v>
@@ -1491,18 +1512,18 @@
         <v>20</v>
       </c>
       <c r="P32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="R32">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -1511,21 +1532,21 @@
         <v>100</v>
       </c>
       <c r="I33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J33" s="2">
         <v>5</v>
       </c>
       <c r="K33" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L33">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1534,9 +1555,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1545,9 +1566,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -1556,9 +1577,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -1567,29 +1588,29 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
       </c>
       <c r="F38">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1598,13 +1619,13 @@
         <v>10</v>
       </c>
       <c r="I39" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J39" s="2">
         <v>2</v>
       </c>
       <c r="K39" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L39">
         <v>-50</v>
@@ -1616,18 +1637,21 @@
         <v>5</v>
       </c>
       <c r="P39" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="R39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1636,21 +1660,21 @@
         <v>10</v>
       </c>
       <c r="I40" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J40" s="2">
         <v>2</v>
       </c>
       <c r="K40" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L40">
         <v>-50</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1659,53 +1683,53 @@
         <v>10</v>
       </c>
       <c r="I41" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J41" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+      <c r="G43" t="s">
+        <v>42</v>
+      </c>
+      <c r="I43" t="s">
+        <v>52</v>
+      </c>
+      <c r="J43" s="2">
+        <v>3</v>
+      </c>
+      <c r="K43" t="s">
         <v>47</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43">
-        <v>10</v>
-      </c>
-      <c r="G43" t="s">
-        <v>46</v>
-      </c>
-      <c r="I43" t="s">
-        <v>56</v>
-      </c>
-      <c r="J43" s="2">
-        <v>3</v>
-      </c>
-      <c r="K43" t="s">
-        <v>51</v>
       </c>
       <c r="L43">
         <v>0</v>
@@ -1717,18 +1741,21 @@
         <v>10</v>
       </c>
       <c r="P43" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q43" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="R43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1737,21 +1764,21 @@
         <v>10</v>
       </c>
       <c r="I44" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J44" s="2">
         <v>3</v>
       </c>
       <c r="K44" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1760,53 +1787,53 @@
         <v>10</v>
       </c>
       <c r="I45" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J45" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47" t="s">
+        <v>42</v>
+      </c>
+      <c r="I47" t="s">
+        <v>57</v>
+      </c>
+      <c r="J47" s="2">
+        <v>3</v>
+      </c>
+      <c r="K47" t="s">
         <v>47</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" t="s">
-        <v>53</v>
-      </c>
-      <c r="D47" t="s">
-        <v>14</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47">
-        <v>10</v>
-      </c>
-      <c r="G47" t="s">
-        <v>46</v>
-      </c>
-      <c r="I47" t="s">
-        <v>61</v>
-      </c>
-      <c r="J47" s="2">
-        <v>3</v>
-      </c>
-      <c r="K47" t="s">
-        <v>51</v>
       </c>
       <c r="L47">
         <v>0</v>
@@ -1818,18 +1845,21 @@
         <v>10</v>
       </c>
       <c r="P47" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q47" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="R47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -1841,15 +1871,15 @@
         <v>3</v>
       </c>
       <c r="K48" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -1861,47 +1891,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>10</v>
+      </c>
+      <c r="G51" t="s">
+        <v>42</v>
+      </c>
+      <c r="I51" t="s">
+        <v>55</v>
+      </c>
+      <c r="J51" s="2">
+        <v>3</v>
+      </c>
+      <c r="K51" t="s">
         <v>47</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>66</v>
-      </c>
-      <c r="B51">
-        <v>2</v>
-      </c>
-      <c r="C51" t="s">
-        <v>66</v>
-      </c>
-      <c r="D51" t="s">
-        <v>14</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51">
-        <v>10</v>
-      </c>
-      <c r="G51" t="s">
-        <v>46</v>
-      </c>
-      <c r="I51" t="s">
-        <v>59</v>
-      </c>
-      <c r="J51" s="2">
-        <v>3</v>
-      </c>
-      <c r="K51" t="s">
-        <v>51</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -1913,18 +1943,21 @@
         <v>10</v>
       </c>
       <c r="P51" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q51" t="s">
         <v>78</v>
       </c>
-      <c r="Q51" t="s">
-        <v>82</v>
-      </c>
       <c r="R51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -1933,21 +1966,21 @@
         <v>10</v>
       </c>
       <c r="I52" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J52" s="2">
         <v>3</v>
       </c>
       <c r="K52" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -1959,9 +1992,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -1970,18 +2003,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B55">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D55" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -1990,16 +2023,16 @@
         <v>50</v>
       </c>
       <c r="G55" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I55" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J55" s="2">
         <v>3</v>
       </c>
       <c r="K55" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L55">
         <v>50</v>
@@ -2011,18 +2044,18 @@
         <v>15</v>
       </c>
       <c r="P55" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q55" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="R55">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E56">
         <v>2</v>
@@ -2031,21 +2064,21 @@
         <v>50</v>
       </c>
       <c r="I56" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J56" s="2">
         <v>3</v>
       </c>
       <c r="K56" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L56">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -2054,15 +2087,15 @@
         <v>10</v>
       </c>
       <c r="I57" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J57" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2071,29 +2104,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>23</v>
-      </c>
-      <c r="E59" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
       </c>
       <c r="F59">
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E60">
         <v>2</v>
@@ -2102,16 +2135,16 @@
         <v>50</v>
       </c>
       <c r="G60" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I60" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J60" s="2">
         <v>3</v>
       </c>
       <c r="K60" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L60">
         <v>50</v>
@@ -2123,18 +2156,18 @@
         <v>15</v>
       </c>
       <c r="P60" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q60" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="R60">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E61">
         <v>2</v>
@@ -2143,21 +2176,21 @@
         <v>50</v>
       </c>
       <c r="I61" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J61" s="2">
         <v>3</v>
       </c>
       <c r="K61" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L61">
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2169,9 +2202,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -2180,12 +2213,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>23</v>
-      </c>
-      <c r="E64" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
       </c>
       <c r="F64">
         <v>25</v>
@@ -2193,16 +2226,16 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B65">
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D65" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E65">
         <v>2</v>
@@ -2211,16 +2244,16 @@
         <v>50</v>
       </c>
       <c r="G65" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I65" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J65" s="2">
         <v>3</v>
       </c>
       <c r="K65" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L65">
         <v>50</v>
@@ -2232,10 +2265,10 @@
         <v>15</v>
       </c>
       <c r="P65" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q65" t="s">
         <v>78</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>82</v>
       </c>
       <c r="R65">
         <v>3</v>
@@ -2243,7 +2276,7 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E66">
         <v>2</v>
@@ -2252,13 +2285,13 @@
         <v>50</v>
       </c>
       <c r="I66" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J66" s="2">
         <v>3</v>
       </c>
       <c r="K66" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L66">
         <v>50</v>
@@ -2266,7 +2299,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -2275,7 +2308,7 @@
         <v>10</v>
       </c>
       <c r="I67" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J67" s="2">
         <v>3</v>
@@ -2283,7 +2316,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -2294,10 +2327,10 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
-        <v>23</v>
-      </c>
-      <c r="E69" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
       </c>
       <c r="F69">
         <v>25</v>

</xml_diff>